<commit_message>
modified doLoginOut.py modified client_app_case.xlsx
</commit_message>
<xml_diff>
--- a/data/client_app_case.xlsx
+++ b/data/client_app_case.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16260"/>
+    <workbookView windowWidth="26960" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="首页" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50">
   <si>
     <t>caseid</t>
   </si>
@@ -41,10 +41,8 @@
   </si>
   <si>
     <t>{
-  "Authorization": "${access_token}",
-  "unionId": "${unionid}",
   "terminalType": "android",
-  "Content-Type": "application/json; charset=utf-8"
+  "Content-Type": "application/json;charset=utf-8"
 }</t>
   </si>
   <si>
@@ -101,15 +99,6 @@
     <t>/appapi/broker/personal/v1/judgeSignInActivity</t>
   </si>
   <si>
-    <t>{
-  "Authorization": "${access_token}",
-  "unionId": "${unionid}",
-  "customerId": "${customerId}",
-  "terminalType": " android",
-  "Content-Type": " application/json; charset=utf-8"
-}</t>
-  </si>
-  <si>
     <t>是否存在签到活动</t>
   </si>
   <si>
@@ -140,13 +129,6 @@
   </si>
   <si>
     <t>{
-  "customerId": "${customerId}",
-  "terminalType": "android",
-  "Content-Type": "application/json; charset=utf-8"
-}</t>
-  </si>
-  <si>
-    <t>{
     "current": 1,
     "size": 5,
     "regionId": "440300"
@@ -232,10 +214,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -260,11 +242,86 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -276,6 +333,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -284,6 +348,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -291,100 +356,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,19 +401,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,37 +527,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,19 +545,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,97 +581,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,11 +630,47 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,6 +679,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -681,203 +710,156 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1243,7 +1225,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" outlineLevelCol="5"/>
@@ -1277,7 +1259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="75" spans="1:6">
+    <row r="2" ht="50" spans="1:6">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1317,7 +1299,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" ht="75" spans="1:6">
+    <row r="4" ht="50" spans="1:6">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1328,7 +1310,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>13</v>
@@ -1348,7 +1330,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>18</v>
@@ -1377,7 +1359,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" ht="100" spans="1:6">
+    <row r="7" ht="50" spans="1:6">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1388,13 +1370,13 @@
         <v>7</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" ht="75" spans="1:6">
@@ -1408,33 +1390,33 @@
         <v>7</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="9" ht="75" spans="1:6">
+    <row r="9" ht="50" spans="1:6">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" ht="62" spans="1:6">
@@ -1442,39 +1424,39 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="11" ht="75" spans="1:6">
+    <row r="11" ht="62" spans="1:6">
       <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" ht="75" spans="1:6">
@@ -1482,19 +1464,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" ht="75" spans="1:6">
@@ -1508,13 +1490,13 @@
         <v>7</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" ht="50" spans="1:6">
@@ -1522,7 +1504,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>7</v>
@@ -1531,10 +1513,10 @@
         <v>12</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" ht="50" spans="1:6">
@@ -1542,7 +1524,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>7</v>
@@ -1551,30 +1533,30 @@
         <v>12</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="16" ht="75" spans="1:6">
+    <row r="16" ht="50" spans="1:6">
       <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>